<commit_message>
add additional raw data for siPHD2 experiments
</commit_message>
<xml_diff>
--- a/data-raw/fluxes/lf_05-siphd/lf_05-siphd_d_2022-11-01.xlsx
+++ b/data-raw/fluxes/lf_05-siphd/lf_05-siphd_d_2022-11-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Dropbox (Partners HealthCare)/_data/Copeland.2022.hypoxia.flux/data-raw/fluxes/lf_05-siphd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Dropbox (Partners HealthCare)/_data/Copeland.2023.hypoxia.flux/data-raw/fluxes/lf_05-siphd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DDCA51-02E4-1146-9178-0048FE87A416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A85C55-5A63-1542-AEE3-739D7A864334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="3880" windowWidth="27140" windowHeight="16940" activeTab="1" xr2:uid="{101A82DF-E6B5-5B46-9986-3500AB660F6E}"/>
+    <workbookView xWindow="2340" yWindow="2780" windowWidth="27140" windowHeight="16940" xr2:uid="{101A82DF-E6B5-5B46-9986-3500AB660F6E}"/>
   </bookViews>
   <sheets>
     <sheet name="evap" sheetId="1" r:id="rId1"/>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -412,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -422,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7685FC2E-8A1C-C645-8D24-132AF64BA898}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE879D2-77E3-EF4E-8F6E-9AEBBCB39BD6}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,13 +592,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>25742</v>
+        <v>44844</v>
       </c>
       <c r="E2">
-        <v>24095</v>
+        <v>39883</v>
       </c>
       <c r="F2">
-        <v>33326</v>
+        <v>41365</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -606,17 +606,17 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C2:C7" si="0">C4/2</f>
+        <f t="shared" ref="C3:C7" si="0">C4/2</f>
         <v>1.5625</v>
       </c>
       <c r="D3">
-        <v>391599</v>
+        <v>1058773</v>
       </c>
       <c r="E3">
-        <v>381220</v>
+        <v>1058660</v>
       </c>
       <c r="F3">
-        <v>399944</v>
+        <v>1014283</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -628,13 +628,13 @@
         <v>3.125</v>
       </c>
       <c r="D4">
-        <v>658947</v>
+        <v>1942830</v>
       </c>
       <c r="E4">
-        <v>711649</v>
+        <v>1929469</v>
       </c>
       <c r="F4">
-        <v>715416</v>
+        <v>1942436</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -646,13 +646,13 @@
         <v>6.25</v>
       </c>
       <c r="D5">
-        <v>1534413</v>
+        <v>3927198</v>
       </c>
       <c r="E5">
-        <v>1469290</v>
+        <v>3791851</v>
       </c>
       <c r="F5">
-        <v>1501032</v>
+        <v>3790873</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -664,13 +664,13 @@
         <v>12.5</v>
       </c>
       <c r="D6">
-        <v>3123930</v>
+        <v>6810676</v>
       </c>
       <c r="E6">
-        <v>3155716</v>
+        <v>7392990</v>
       </c>
       <c r="F6">
-        <v>2743292</v>
+        <v>7307346</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -682,13 +682,13 @@
         <v>25</v>
       </c>
       <c r="D7">
-        <v>6155243</v>
+        <v>14981559</v>
       </c>
       <c r="E7">
-        <v>5797157</v>
+        <v>14346887</v>
       </c>
       <c r="F7">
-        <v>5753309</v>
+        <v>14270570</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -700,13 +700,13 @@
         <v>50</v>
       </c>
       <c r="D8">
-        <v>11590018</v>
+        <v>30379368</v>
       </c>
       <c r="E8">
-        <v>11499904</v>
+        <v>28899010</v>
       </c>
       <c r="F8">
-        <v>10318691</v>
+        <v>29143216</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -717,13 +717,13 @@
         <v>100</v>
       </c>
       <c r="D9">
-        <v>25396706</v>
+        <v>64868556</v>
       </c>
       <c r="E9">
-        <v>22812188</v>
+        <v>59817952</v>
       </c>
       <c r="F9">
-        <v>22512156</v>
+        <v>62458144</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -734,13 +734,13 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>576126</v>
+        <v>2133066</v>
       </c>
       <c r="E10">
-        <v>715642</v>
+        <v>2188183</v>
       </c>
       <c r="F10">
-        <v>497929</v>
+        <v>1916836</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -752,13 +752,13 @@
         <v>2</v>
       </c>
       <c r="D11">
-        <v>552765</v>
+        <v>1091172</v>
       </c>
       <c r="E11">
-        <v>891330</v>
+        <v>1771933</v>
       </c>
       <c r="F11">
-        <v>756771</v>
+        <v>1364459</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -766,17 +766,17 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:B75" si="1">1+B11</f>
+        <f t="shared" ref="B12:B57" si="1">1+B11</f>
         <v>3</v>
       </c>
       <c r="D12">
-        <v>710257</v>
+        <v>1106769</v>
       </c>
       <c r="E12">
-        <v>1063610</v>
+        <v>1329995</v>
       </c>
       <c r="F12">
-        <v>821490</v>
+        <v>1441278</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -788,13 +788,13 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>930815</v>
+        <v>2600588</v>
       </c>
       <c r="E13">
-        <v>883000</v>
+        <v>2505965</v>
       </c>
       <c r="F13">
-        <v>833870</v>
+        <v>2039369</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -806,13 +806,13 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>893630</v>
+        <v>1648064</v>
       </c>
       <c r="E14">
-        <v>1111522</v>
+        <v>1669353</v>
       </c>
       <c r="F14">
-        <v>1117473</v>
+        <v>2459277</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -824,13 +824,13 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <v>1058849</v>
+        <v>2494961</v>
       </c>
       <c r="E15">
-        <v>1009038</v>
+        <v>1984960</v>
       </c>
       <c r="F15">
-        <v>934242</v>
+        <v>2646266</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -842,13 +842,13 @@
         <v>7</v>
       </c>
       <c r="D16">
-        <v>681368</v>
+        <v>1547056</v>
       </c>
       <c r="E16">
-        <v>683346</v>
+        <v>1266249</v>
       </c>
       <c r="F16">
-        <v>825352</v>
+        <v>1148969</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -860,13 +860,13 @@
         <v>8</v>
       </c>
       <c r="D17">
-        <v>384241</v>
+        <v>955681</v>
       </c>
       <c r="E17">
-        <v>320648</v>
+        <v>774627</v>
       </c>
       <c r="F17">
-        <v>320047</v>
+        <v>1232056</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -878,13 +878,13 @@
         <v>9</v>
       </c>
       <c r="D18">
-        <v>883555</v>
+        <v>1621711</v>
       </c>
       <c r="E18">
-        <v>696177</v>
+        <v>1048805</v>
       </c>
       <c r="F18">
-        <v>680325</v>
+        <v>1198937</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -896,13 +896,13 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>835173</v>
+        <v>1268150</v>
       </c>
       <c r="E19">
-        <v>694630</v>
+        <v>1562443</v>
       </c>
       <c r="F19">
-        <v>730453</v>
+        <v>1517336</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -914,13 +914,13 @@
         <v>11</v>
       </c>
       <c r="D20">
-        <v>966911</v>
+        <v>1509414</v>
       </c>
       <c r="E20">
-        <v>729012</v>
+        <v>1447800</v>
       </c>
       <c r="F20">
-        <v>585800</v>
+        <v>1520465</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -932,13 +932,13 @@
         <v>12</v>
       </c>
       <c r="D21">
-        <v>1071104</v>
+        <v>1140904</v>
       </c>
       <c r="E21">
-        <v>745844</v>
+        <v>1623929</v>
       </c>
       <c r="F21">
-        <v>446704</v>
+        <v>1388622</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -950,13 +950,13 @@
         <v>13</v>
       </c>
       <c r="D22">
-        <v>1150616</v>
+        <v>3454268</v>
       </c>
       <c r="E22">
-        <v>1279851</v>
+        <v>3815123</v>
       </c>
       <c r="F22">
-        <v>1373244</v>
+        <v>3646638</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -968,13 +968,13 @@
         <v>14</v>
       </c>
       <c r="D23">
-        <v>1800898</v>
+        <v>4335980</v>
       </c>
       <c r="E23">
-        <v>1819213</v>
+        <v>3867928</v>
       </c>
       <c r="F23">
-        <v>1577432</v>
+        <v>3695343</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -986,13 +986,13 @@
         <v>15</v>
       </c>
       <c r="D24">
-        <v>1112285</v>
+        <v>4337564</v>
       </c>
       <c r="E24">
-        <v>1446868</v>
+        <v>3642288</v>
       </c>
       <c r="F24">
-        <v>2015168</v>
+        <v>3647120</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1004,13 +1004,13 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>1987592</v>
+        <v>3414844</v>
       </c>
       <c r="E25">
-        <v>1731964</v>
+        <v>3771788</v>
       </c>
       <c r="F25">
-        <v>1947228</v>
+        <v>3961920</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1022,13 +1022,13 @@
         <v>17</v>
       </c>
       <c r="D26">
-        <v>1675856</v>
+        <v>3392548</v>
       </c>
       <c r="E26">
-        <v>2054176</v>
+        <v>3585619</v>
       </c>
       <c r="F26">
-        <v>2169878</v>
+        <v>3807008</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1040,13 +1040,13 @@
         <v>18</v>
       </c>
       <c r="D27">
-        <v>1667326</v>
+        <v>4072605</v>
       </c>
       <c r="E27">
-        <v>1800316</v>
+        <v>3943070</v>
       </c>
       <c r="F27">
-        <v>2488303</v>
+        <v>3869258</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1058,13 +1058,13 @@
         <v>19</v>
       </c>
       <c r="D28">
-        <v>962019</v>
+        <v>2149766</v>
       </c>
       <c r="E28">
-        <v>1027569</v>
+        <v>2099665</v>
       </c>
       <c r="F28">
-        <v>1446906</v>
+        <v>2079078</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1076,13 +1076,13 @@
         <v>20</v>
       </c>
       <c r="D29">
-        <v>1601970</v>
+        <v>2387648</v>
       </c>
       <c r="E29">
-        <v>1303951</v>
+        <v>1510600</v>
       </c>
       <c r="F29">
-        <v>1239426</v>
+        <v>1855310</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1094,13 +1094,13 @@
         <v>21</v>
       </c>
       <c r="D30">
-        <v>1353698</v>
+        <v>1717265</v>
       </c>
       <c r="E30">
-        <v>1190026</v>
+        <v>2143006</v>
       </c>
       <c r="F30">
-        <v>942785</v>
+        <v>2793991</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1112,13 +1112,13 @@
         <v>22</v>
       </c>
       <c r="D31">
-        <v>1113833</v>
+        <v>2036174</v>
       </c>
       <c r="E31">
-        <v>1196656</v>
+        <v>2107250</v>
       </c>
       <c r="F31">
-        <v>1467523</v>
+        <v>2682724</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1130,13 +1130,13 @@
         <v>23</v>
       </c>
       <c r="D32">
-        <v>1348461</v>
+        <v>2044288</v>
       </c>
       <c r="E32">
-        <v>1160766</v>
+        <v>2254020</v>
       </c>
       <c r="F32">
-        <v>1070897</v>
+        <v>2250797</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1148,13 +1148,13 @@
         <v>24</v>
       </c>
       <c r="D33">
-        <v>846695</v>
+        <v>2013578</v>
       </c>
       <c r="E33">
-        <v>509525</v>
+        <v>2224121</v>
       </c>
       <c r="F33">
-        <v>383786</v>
+        <v>2304648</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1166,13 +1166,13 @@
         <v>25</v>
       </c>
       <c r="D34">
-        <v>2369991</v>
+        <v>6352604</v>
       </c>
       <c r="E34">
-        <v>2307400</v>
+        <v>5799052</v>
       </c>
       <c r="F34">
-        <v>2268992</v>
+        <v>5876998</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1184,13 +1184,13 @@
         <v>26</v>
       </c>
       <c r="D35">
-        <v>2805782</v>
+        <v>5467045</v>
       </c>
       <c r="E35">
-        <v>2590854</v>
+        <v>5401330</v>
       </c>
       <c r="F35">
-        <v>2158252</v>
+        <v>6047687</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1202,13 +1202,13 @@
         <v>27</v>
       </c>
       <c r="D36">
-        <v>3264236</v>
+        <v>5573839</v>
       </c>
       <c r="E36">
-        <v>2651682</v>
+        <v>5969860</v>
       </c>
       <c r="F36">
-        <v>2829678</v>
+        <v>6258988</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1220,13 +1220,13 @@
         <v>28</v>
       </c>
       <c r="D37">
-        <v>3231528</v>
+        <v>6074824</v>
       </c>
       <c r="E37">
-        <v>2540303</v>
+        <v>5657978</v>
       </c>
       <c r="F37">
-        <v>3259533</v>
+        <v>6895222</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1238,13 +1238,13 @@
         <v>29</v>
       </c>
       <c r="D38">
-        <v>2528348</v>
+        <v>6709402</v>
       </c>
       <c r="E38">
-        <v>2369636</v>
+        <v>6107761</v>
       </c>
       <c r="F38">
-        <v>2650254</v>
+        <v>5974299</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1256,13 +1256,13 @@
         <v>30</v>
       </c>
       <c r="D39">
-        <v>2549196</v>
+        <v>7127276</v>
       </c>
       <c r="E39">
-        <v>2674364</v>
+        <v>5717771</v>
       </c>
       <c r="F39">
-        <v>3033770</v>
+        <v>5819718</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -1274,13 +1274,13 @@
         <v>31</v>
       </c>
       <c r="D40">
-        <v>2025338</v>
+        <v>3835153</v>
       </c>
       <c r="E40">
-        <v>1759503</v>
+        <v>3385333</v>
       </c>
       <c r="F40">
-        <v>1767249</v>
+        <v>3891562</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -1292,13 +1292,13 @@
         <v>32</v>
       </c>
       <c r="D41">
-        <v>2926257</v>
+        <v>3946717</v>
       </c>
       <c r="E41">
-        <v>1744201</v>
+        <v>3153668</v>
       </c>
       <c r="F41">
-        <v>1929354</v>
+        <v>3887459</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -1310,13 +1310,13 @@
         <v>33</v>
       </c>
       <c r="D42">
-        <v>2072026</v>
+        <v>4584600</v>
       </c>
       <c r="E42">
-        <v>1712539</v>
+        <v>3819513</v>
       </c>
       <c r="F42">
-        <v>1823882</v>
+        <v>3795733</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -1328,13 +1328,13 @@
         <v>34</v>
       </c>
       <c r="D43">
-        <v>2039062</v>
+        <v>4247594</v>
       </c>
       <c r="E43">
-        <v>2050333</v>
+        <v>4264192</v>
       </c>
       <c r="F43">
-        <v>1912358</v>
+        <v>3667922</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -1346,13 +1346,13 @@
         <v>35</v>
       </c>
       <c r="D44">
-        <v>1957630</v>
+        <v>3214305</v>
       </c>
       <c r="E44">
-        <v>2518321</v>
+        <v>3753536</v>
       </c>
       <c r="F44">
-        <v>2460022</v>
+        <v>3610741</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -1364,13 +1364,13 @@
         <v>36</v>
       </c>
       <c r="D45">
-        <v>2019627</v>
+        <v>3227108</v>
       </c>
       <c r="E45">
-        <v>1526191</v>
+        <v>3512434</v>
       </c>
       <c r="F45">
-        <v>2247808</v>
+        <v>3796065</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -1382,13 +1382,13 @@
         <v>37</v>
       </c>
       <c r="D46">
-        <v>3597697</v>
+        <v>7365754</v>
       </c>
       <c r="E46">
-        <v>3978099</v>
+        <v>7615056</v>
       </c>
       <c r="F46">
-        <v>3440024</v>
+        <v>7610168</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -1400,13 +1400,13 @@
         <v>38</v>
       </c>
       <c r="D47">
-        <v>3004060</v>
+        <v>7675102</v>
       </c>
       <c r="E47">
-        <v>3627642</v>
+        <v>7408166</v>
       </c>
       <c r="F47">
-        <v>3166189</v>
+        <v>6502960</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -1418,13 +1418,13 @@
         <v>39</v>
       </c>
       <c r="D48">
-        <v>2785741</v>
+        <v>6394916</v>
       </c>
       <c r="E48">
-        <v>2619313</v>
+        <v>6087944</v>
       </c>
       <c r="F48">
-        <v>2630874</v>
+        <v>6723658</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1436,13 +1436,13 @@
         <v>40</v>
       </c>
       <c r="D49">
-        <v>2427290</v>
+        <v>5861176</v>
       </c>
       <c r="E49">
-        <v>2548024</v>
+        <v>5595772</v>
       </c>
       <c r="F49">
-        <v>2157452</v>
+        <v>5255994</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -1454,13 +1454,13 @@
         <v>41</v>
       </c>
       <c r="D50">
-        <v>3584404</v>
+        <v>8071938</v>
       </c>
       <c r="E50">
-        <v>3628352</v>
+        <v>7979796</v>
       </c>
       <c r="F50">
-        <v>3993116</v>
+        <v>9742366</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -1472,13 +1472,13 @@
         <v>42</v>
       </c>
       <c r="D51">
-        <v>3704112</v>
+        <v>9368005</v>
       </c>
       <c r="E51">
-        <v>3510371</v>
+        <v>8806751</v>
       </c>
       <c r="F51">
-        <v>3994682</v>
+        <v>8545450</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -1490,13 +1490,13 @@
         <v>43</v>
       </c>
       <c r="D52">
-        <v>2458391</v>
+        <v>5084557</v>
       </c>
       <c r="E52">
-        <v>2734665</v>
+        <v>5153976</v>
       </c>
       <c r="F52">
-        <v>2792889</v>
+        <v>5448598</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -1508,13 +1508,13 @@
         <v>44</v>
       </c>
       <c r="D53">
-        <v>2293320</v>
+        <v>4227734</v>
       </c>
       <c r="E53">
-        <v>3009620</v>
+        <v>5167980</v>
       </c>
       <c r="F53">
-        <v>2311577</v>
+        <v>4467764</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -1526,13 +1526,13 @@
         <v>45</v>
       </c>
       <c r="D54">
-        <v>1945575</v>
+        <v>4587386</v>
       </c>
       <c r="E54">
-        <v>4268447</v>
+        <v>4173160</v>
       </c>
       <c r="F54">
-        <v>2838561</v>
+        <v>4726405</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -1544,13 +1544,13 @@
         <v>46</v>
       </c>
       <c r="D55">
-        <v>2380290</v>
+        <v>5440007</v>
       </c>
       <c r="E55">
-        <v>2850300</v>
+        <v>4662962</v>
       </c>
       <c r="F55">
-        <v>2729245</v>
+        <v>4261628</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -1562,13 +1562,13 @@
         <v>47</v>
       </c>
       <c r="D56">
-        <v>3224096</v>
+        <v>4522908</v>
       </c>
       <c r="E56">
-        <v>2856198</v>
+        <v>4512170</v>
       </c>
       <c r="F56">
-        <v>3994022</v>
+        <v>4653296</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -1580,13 +1580,13 @@
         <v>48</v>
       </c>
       <c r="D57">
-        <v>2776324</v>
+        <v>4543330</v>
       </c>
       <c r="E57">
-        <v>2854484</v>
+        <v>4508427</v>
       </c>
       <c r="F57">
-        <v>3232572</v>
+        <v>4267226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>